<commit_message>
Gonzalo: cambios para informe de evaluadores
</commit_message>
<xml_diff>
--- a/Tarea/DataTarea_Exogenas.xlsx
+++ b/Tarea/DataTarea_Exogenas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\CUECOPolMon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2663\Documents\GitHub\CUECOPolMon\Tarea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C44565-AFE0-46D2-9DF6-0A156EA3B39F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1434F39-3D2C-4A78-B526-7537B7DEA393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{AA418475-98CD-40C4-9F54-B699117667D7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AA418475-98CD-40C4-9F54-B699117667D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Uvar" sheetId="1" r:id="rId1"/>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
-  <si>
-    <t>Meta</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>DYs</t>
   </si>
@@ -60,9 +57,6 @@
     <t>Dps</t>
   </si>
   <si>
-    <t>Dpms</t>
-  </si>
-  <si>
     <t>iext</t>
   </si>
   <si>
@@ -72,18 +66,12 @@
     <t>res_ys</t>
   </si>
   <si>
-    <t>res_Dpms</t>
-  </si>
-  <si>
     <t>res_iext</t>
   </si>
   <si>
     <t>res_DTI</t>
   </si>
   <si>
-    <t>res_Meta</t>
-  </si>
-  <si>
     <t>res_g</t>
   </si>
   <si>
@@ -94,6 +82,9 @@
   </si>
   <si>
     <t>res_DYs_eq</t>
+  </si>
+  <si>
+    <t>ys</t>
   </si>
 </sst>
 </file>
@@ -540,83 +531,77 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>45747</v>
       </c>
       <c r="B3" s="7">
-        <v>2</v>
+        <v>2.2079178189177071</v>
       </c>
       <c r="C3" s="7">
-        <v>2.2079178189177071</v>
+        <v>-0.30513363517802289</v>
       </c>
       <c r="D3" s="7">
         <v>2.987567660193188</v>
@@ -633,22 +618,19 @@
       <c r="H3" s="7">
         <v>1.384126466184451</v>
       </c>
-      <c r="I3" s="7">
-        <v>1.192761245670694</v>
-      </c>
-      <c r="J3" s="9">
+      <c r="I3" s="9">
         <v>0.66384956126651085</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>45838</v>
       </c>
       <c r="B4" s="7">
-        <v>2</v>
+        <v>1.9757863828806661</v>
       </c>
       <c r="C4" s="7">
-        <v>1.9757863828806661</v>
+        <v>-0.17154856357227169</v>
       </c>
       <c r="D4" s="7">
         <v>1.998146564230074</v>
@@ -665,22 +647,19 @@
       <c r="H4" s="7">
         <v>1.5930540365912851</v>
       </c>
-      <c r="I4" s="7">
-        <v>1.551268522509919</v>
-      </c>
-      <c r="J4" s="9">
+      <c r="I4" s="9">
         <v>0.87667017433157601</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>45930</v>
       </c>
       <c r="B5" s="7">
-        <v>2</v>
+        <v>1.781166667338816</v>
       </c>
       <c r="C5" s="7">
-        <v>1.781166667338816</v>
+        <v>-8.8264805610846986E-2</v>
       </c>
       <c r="D5" s="7">
         <v>2.0005524745618741</v>
@@ -697,22 +676,19 @@
       <c r="H5" s="7">
         <v>1.6468334275879011</v>
       </c>
-      <c r="I5" s="7">
-        <v>1.636077549388578</v>
-      </c>
-      <c r="J5" s="9">
+      <c r="I5" s="9">
         <v>1.0455613233791039</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>46022</v>
       </c>
       <c r="B6" s="7">
-        <v>2</v>
+        <v>1.6404176706355009</v>
       </c>
       <c r="C6" s="7">
-        <v>1.6404176706355009</v>
+        <v>-4.1798217736525048E-2</v>
       </c>
       <c r="D6" s="7">
         <v>2.034654816605586</v>
@@ -729,22 +705,19 @@
       <c r="H6" s="7">
         <v>1.664769343392815</v>
       </c>
-      <c r="I6" s="7">
-        <v>1.6611821602318331</v>
-      </c>
-      <c r="J6" s="9">
+      <c r="I6" s="9">
         <v>1.174829384708675</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>46112</v>
       </c>
       <c r="B7" s="7">
-        <v>2</v>
+        <v>1.5465767365636569</v>
       </c>
       <c r="C7" s="7">
-        <v>1.5465767365636569</v>
+        <v>-2.0405485082324409E-2</v>
       </c>
       <c r="D7" s="7">
         <v>2.0588353026717501</v>
@@ -761,22 +734,19 @@
       <c r="H7" s="7">
         <v>1.672242801530579</v>
       </c>
-      <c r="I7" s="7">
-        <v>1.6707481099030259</v>
-      </c>
-      <c r="J7" s="9">
+      <c r="I7" s="9">
         <v>1.270894955175071</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>46203</v>
       </c>
       <c r="B8" s="7">
-        <v>2</v>
+        <v>1.4889754055932769</v>
       </c>
       <c r="C8" s="7">
-        <v>1.4889754055932769</v>
+        <v>-1.5010570655856009E-2</v>
       </c>
       <c r="D8" s="7">
         <v>2.084969551106191</v>
@@ -793,22 +763,19 @@
       <c r="H8" s="7">
         <v>1.6756188688010101</v>
       </c>
-      <c r="I8" s="7">
-        <v>1.6749436553469239</v>
-      </c>
-      <c r="J8" s="9">
+      <c r="I8" s="9">
         <v>1.340408717430285</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>46295</v>
       </c>
       <c r="B9" s="7">
-        <v>2</v>
+        <v>1.4577046178661319</v>
       </c>
       <c r="C9" s="7">
-        <v>1.4577046178661319</v>
+        <v>-1.9014863791458721E-2</v>
       </c>
       <c r="D9" s="7">
         <v>2.103785520902214</v>
@@ -825,22 +792,19 @@
       <c r="H9" s="7">
         <v>1.6771042002492009</v>
       </c>
-      <c r="I9" s="7">
-        <v>1.676807133959564</v>
-      </c>
-      <c r="J9" s="9">
+      <c r="I9" s="9">
         <v>1.3894703557769941</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>46387</v>
       </c>
       <c r="B10" s="7">
-        <v>2</v>
+        <v>1.4446280052340581</v>
       </c>
       <c r="C10" s="7">
-        <v>1.4446280052340581</v>
+        <v>-2.7854005609061039E-2</v>
       </c>
       <c r="D10" s="7">
         <v>2.1122113640225701</v>
@@ -857,10 +821,7 @@
       <c r="H10" s="7">
         <v>1.6777659436680299</v>
       </c>
-      <c r="I10" s="7">
-        <v>1.6776335949842649</v>
-      </c>
-      <c r="J10" s="9">
+      <c r="I10" s="9">
         <v>1.423303583980273</v>
       </c>
     </row>
@@ -878,32 +839,32 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>45717</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>45809</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>45901</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>45992</v>
       </c>

</xml_diff>